<commit_message>
add row by alaaeddin
</commit_message>
<xml_diff>
--- a/Init.xlsx
+++ b/Init.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Title</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Changed data</t>
+  </si>
+  <si>
+    <t>This row was added by branch Alaaeddin</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -376,7 +379,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -399,7 +402,12 @@
       </c>
       <c r="B3" s="1">
         <f ca="1">NOW()</f>
-        <v>42348.769832754631</v>
+        <v>42348.805635648147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a new sheet
</commit_message>
<xml_diff>
--- a/Init.xlsx
+++ b/Init.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Alaaeddin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Title</t>
   </si>
@@ -29,6 +30,9 @@
   </si>
   <si>
     <t>This row was added by branch Alaaeddin</t>
+  </si>
+  <si>
+    <t>Data added by Alaaeddin branch</t>
   </si>
 </sst>
 </file>
@@ -373,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,12 +406,32 @@
       </c>
       <c r="B3" s="1">
         <f ca="1">NOW()</f>
-        <v>42348.805635648147</v>
+        <v>42348.812421527778</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>